<commit_message>
docs: some further result processing
</commit_message>
<xml_diff>
--- a/results/ProcessingResults.xlsx
+++ b/results/ProcessingResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Libraries\Documents\School\Y2\Term 3\Ad. Tools Unfam\Game-Engine-Performance-In-VR\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{38C2774F-8BBD-4223-8AA8-ED85B3465EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4842A7FD-EFDA-47BB-B77A-04CF122CB6A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{65462524-CA69-4EC5-8A75-82FCA1BF4F2E}"/>
   </bookViews>
@@ -828,7 +828,7 @@
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Analysis!$D$4</c:f>
@@ -971,13 +971,13 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1FCE-49B8-98C2-FD3EF302DD9D}"/>
+              <c16:uniqueId val="{00000001-74FB-42AF-92D6-64567AB231C7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>Analysis!$E$4</c:f>
@@ -1120,7 +1120,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1FCE-49B8-98C2-FD3EF302DD9D}"/>
+              <c16:uniqueId val="{00000003-74FB-42AF-92D6-64567AB231C7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1134,6 +1134,348 @@
         </c:dLbls>
         <c:axId val="611605248"/>
         <c:axId val="611830208"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Analysis!$D$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Frame Rate Unity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent3">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="3"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="60000"/>
+                        <a:lumOff val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:glow rad="63500">
+                        <a:schemeClr val="accent3">
+                          <a:satMod val="175000"/>
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:glow>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Analysis!$B$5:$B$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>400</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Analysis!$D$5:$D$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>71.900000000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>62.3</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>36</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>24</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>18</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>18</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-74FB-42AF-92D6-64567AB231C7}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Analysis!$E$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v> Frame Rate Unreal</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:glow rad="139700">
+                      <a:schemeClr val="accent4">
+                        <a:satMod val="175000"/>
+                        <a:alpha val="14000"/>
+                      </a:schemeClr>
+                    </a:glow>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="3"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="60000"/>
+                        <a:lumOff val="40000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst>
+                      <a:glow rad="63500">
+                        <a:schemeClr val="accent4">
+                          <a:satMod val="175000"/>
+                          <a:alpha val="25000"/>
+                        </a:schemeClr>
+                      </a:glow>
+                    </a:effectLst>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Analysis!$B$5:$B$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>200</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>400</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>1500</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2500</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>3000</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>3500</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Analysis!$E$5:$E$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00</c:formatCode>
+                      <c:ptCount val="12"/>
+                      <c:pt idx="0">
+                        <c:v>72</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>70</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>66.400000000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>47.8</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>35</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>23.8</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>13.8</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>9.8000000000000007</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>8.8000000000000007</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>7.2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>6.2</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>5.4</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-74FB-42AF-92D6-64567AB231C7}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="611605248"/>
@@ -1221,8 +1563,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1300,8 +1643,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.3423423755741274E-2"/>
-              <c:y val="0.45035718670180963"/>
+              <c:x val="1.4332657920556937E-2"/>
+              <c:y val="0.44730582153973303"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1944,8 +2287,9 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:noFill/>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2178,6 +2522,709 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Frame rate comparison Unity vs Unreal</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analysis!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Frame Rate Unity</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analysis!$B$5:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analysis!$D$5:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>71.900000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FEFE-4F47-ABCC-C1E8AB7FCAB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Analysis!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v> Frame Rate Unreal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Analysis!$B$5:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Analysis!$E$5:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FEFE-4F47-ABCC-C1E8AB7FCAB0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="611605248"/>
+        <c:axId val="611830208"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="611605248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Objects</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> in the scene</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611830208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="611830208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Frame Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.4332657920556937E-2"/>
+              <c:y val="0.44730582153973303"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="611605248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln cap="rnd">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:lumMod val="15000"/>
+              <a:lumOff val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="rnd" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2258,6 +3305,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
@@ -3334,20 +4421,558 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>15178</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>10714</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>569361</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>166577</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>593911</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>541957</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3375,15 +5000,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>12425</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>3311</xdr:rowOff>
+      <xdr:colOff>202925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>107220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>110021</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3408,7 +5033,510 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>478782</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>147871</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C72D7E9-CEEF-4473-B500-B18098AF0826}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>499933</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>31500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>325307</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>141180</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="17" name="Ink 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{367D3CA0-1401-3918-2F55-B8E733F8C8B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="5320411" y="10716065"/>
+            <a:ext cx="1051200" cy="490680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="17" name="Ink 16">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{367D3CA0-1401-3918-2F55-B8E733F8C8B2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5314291" y="10709945"/>
+              <a:ext cx="1063440" cy="502920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304041</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>146760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>17788</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>58680</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="18" name="Ink 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8664F34E-14DE-B0BC-90B8-73A5950F5451}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7576171" y="10640825"/>
+            <a:ext cx="2165400" cy="673920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="18" name="Ink 17">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8664F34E-14DE-B0BC-90B8-73A5950F5451}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7570014" y="10634705"/>
+              <a:ext cx="2177714" cy="686160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>278867</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>66000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200888</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>149700</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="20" name="Ink 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB574316-1134-C54F-897C-BC121989A2D4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6325171" y="10941065"/>
+            <a:ext cx="1760760" cy="1798200"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="20" name="Ink 19">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB574316-1134-C54F-897C-BC121989A2D4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6319051" y="10934945"/>
+              <a:ext cx="1773000" cy="1810440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>158188</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>5820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>547489</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>42540</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FAFA199-0B4C-1FC2-1F72-60CE908442B4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9881971" y="11071385"/>
+            <a:ext cx="2228040" cy="1179720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="22" name="Ink 21">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FAFA199-0B4C-1FC2-1F72-60CE908442B4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9875851" y="11065265"/>
+              <a:ext cx="2240280" cy="1191960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>372587</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>8160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>372947</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>8520</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296F78DD-3638-CDBD-A390-76CD6B1EF3E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="3751891" y="9359225"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="23" name="Ink 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296F78DD-3638-CDBD-A390-76CD6B1EF3E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3745771" y="9353105"/>
+              <a:ext cx="12600" cy="12600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-06-12T13:35:48.239"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFC114"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">130 96 24575,'2'9'0,"-1"-1"0,2 0 0,-1 0 0,1 0 0,0 0 0,1 0 0,0 0 0,0-1 0,7 9 0,6 12 0,13 22 0,2-1 0,43 49 0,-4-4 0,-48-65 0,2-2 0,44 40 0,-10-11 0,-33-34 0,1 0 0,2-2 0,40 23 0,-49-31 0,126 72 0,-117-69 0,0-2 0,44 15 0,-41-17 0,0 1 0,31 18 0,84 35 0,62 36 0,-170-83 0,226 82 0,-134-47 0,-98-44 0,1-2 0,0-1 0,0-1 0,52 0 0,-13-7 0,108-15 0,-20-2 0,-91 13 0,7-1 0,-71 5 0,-1 1 0,1-1 0,0 0 0,-1 0 0,0 0 0,1-1 0,-1 0 0,0 0 0,0-1 0,8-7 0,2-3 0,-7 7 0,0 1 0,0-2 0,-1 1 0,0-1 0,0 0 0,-1-1 0,0 1 0,-1-1 0,1-1 0,-2 1 0,1-1 0,-2 1 0,6-19 0,12-111 0,-17 115 0,-1 0 0,-1 0 0,-1-1 0,-1 1 0,-1 0 0,-1 0 0,-1-1 0,-11-38 0,10 55 0,-1 1 0,1-1 0,-2 1 0,1 0 0,-1 1 0,0-1 0,0 1 0,-1 0 0,0 1 0,0-1 0,-11-5 0,-31-28 0,26 20 0,0 0 0,-34-20 0,-13-10 0,-40-26 0,89 62 0,-1 1 0,-1 1 0,0 0 0,0 2 0,-1 1 0,0 1 0,-38-6 0,12 2 0,-111-12 0,62 5 0,-45-11 0,143 29 0,-32-10 0,-1 1 0,-37-4 0,-67-10 0,0 1 0,125 19 0,-1 0 0,1-1 0,-23-9 0,25 9 0,0-1 0,-1 2 0,1-1 0,-1 2 0,-17-3 0,-60-9 0,40 5 0,19 3 0,0-2 0,-44-17 0,15 4 0,27 13 0,1 0 0,-1 2 0,0 1 0,-39-1 0,39 4 0,0 2 0,0 0 0,-1 2 0,1 2 0,0 1 0,0 1 0,-34 12 0,0-2 0,54-15 0,1 1 0,-1 1 0,1 0 0,-1 0 0,-11 6 0,-26 14 0,-40 23 0,40-20 56,38-22-340,1 1 0,0 0-1,0 1 1,-18 14 0,18-10-6542</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-06-12T13:35:52.758"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#FFC114"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">52 122 24575,'0'55'0,"-1"-13"0,5 54 0,-2-82 0,0 0 0,1 0 0,1-1 0,0 1 0,0-1 0,2 0 0,12 23 0,-11-21 0,0 0 0,0 1 0,-1 0 0,5 24 0,-7-22 0,1-1 0,1 0 0,15 31 0,2-5 0,21 52 0,-5-20 0,-28-58 0,-2 1 0,0 0 0,8 22 0,-9-19 0,1-1 0,1-1 0,14 23 0,12 22 0,-27-49 0,-1 0 0,2-1 0,0 0 0,1 0 0,0-1 0,1-1 0,21 17 0,8 4 0,51 30 0,-69-52 0,0 0 0,1-2 0,0 0 0,0-1 0,1-2 0,-1-1 0,1 0 0,33 0 0,-44-2 0,-1 0 0,0 0 0,23 10 0,-24-8 0,-1-1 0,1 0 0,0-1 0,0 0 0,14 1 0,55 8 0,-56-7 0,1-2 0,25 1 0,7-1 0,98 19 0,7 0 0,-54-10 0,139 34 0,-47-16 0,-175-27 0,13 4 0,0 1 0,40 14 0,40 9 0,36-3 0,-17 12 0,-101-31 0,-17-4 0,-1-1 0,1-1 0,24 1 0,65 8 0,-73-7 0,48 1 0,808-7 0,-875 2 0,0 1 0,31 7 0,30 3 0,-10-12 0,-38-1 0,0 2 0,0 1 0,50 9 0,-41-5 0,0-1 0,1-2 0,-1-2 0,46-4 0,7 0 0,-4 1 0,98 5 0,-118 8 0,-47-7 0,0-1 0,29 2 0,29-4 0,139-4 0,-208 1 0,0 0 0,-1 0 0,1-1 0,-1-1 0,0 0 0,0 0 0,12-8 0,57-42 0,-62 40 0,0-1 0,0 0 0,-2-1 0,0-1 0,-1 0 0,0-1 0,-1 0 0,-2-1 0,13-29 0,-17 38 0,0 1 0,0-1 0,1 1 0,0 0 0,8-8 0,-8 9 0,0 1 0,0-1 0,-1-1 0,0 1 0,-1-1 0,6-12 0,9-22 0,-13 31 0,-2 0 0,1-1 0,4-19 0,-2 2 0,-3 12 0,-1 0 0,0 0 0,0-18 0,-3 30 0,-1 0 0,0 1 0,-1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,-7-7 0,-131-160 0,135 168 0,-25-29 0,-41-37 0,-8-10 0,50 60 0,-1 2 0,0 1 0,-1 1 0,-1 1 0,-59-18 0,10 2 0,26 12 0,0 3 0,-107-18 0,145 32 0,-55-19 0,57 16 0,0 1 0,-1 0 0,-26-3 0,-118-18 0,97 16 0,32 5 0,-58-2 0,-49-5 0,0 1 0,117 10 0,0-1 0,-28-7 0,27 5 0,0 1 0,-25-1 0,12 2 0,-63-11 0,88 11 0,-20-2 0,-45 1 0,50 3 0,0-2 0,0 0 0,-28-6 0,26 3 0,0 2 0,0 0 0,-1 2 0,-35 3 0,-52-2 0,46-11 0,48 7 0,0 0 0,-28 0 0,-51 6 0,-75-4 0,107-9 0,48 7 0,0 0 0,-32-1 0,-50-6 0,72 6 0,-44-1 0,40 4 0,-51-10 0,21 2 0,41 6 0,1-1 0,-27-9 0,-40-9 0,-139-23 0,205 42 0,1-2 0,0 0 0,-28-12 0,10 3 0,19 9 0,-1 1 0,0 2 0,0 0 0,-1 1 0,-24 1 0,19 1 0,1-2 0,-49-8 0,45 5 0,0 1 0,0 2 0,-1 1 0,-38 3 0,26 0 0,-50-4 0,32-9 0,-13-1 0,-12 0 0,63 8 0,-48-3 0,39 7 0,5 0 0,1 0 0,-1-2 0,-49-9 0,51 5 0,-1 2 0,1 1 0,-1 1 0,0 2 0,1 0 0,-1 2 0,-29 5 0,34 0 0,1 1 0,-1 0 0,2 2 0,-39 23 0,16-9 0,1 2 0,1 2 0,1 1 0,-55 54 0,47-17-1365,38-56-5461</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-06-12T13:36:07.577"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">100 1 24575,'-2'7'0,"0"0"0,0 0 0,0 0 0,-1-1 0,-4 9 0,0 0 0,-23 83 0,6-15 0,18-57 0,1-1 0,1 1 0,1 0 0,1 1 0,2-1 0,4 46 0,-1 8 0,-5 18 0,4 103 0,9-133 0,-6-47 0,-2 1 0,1 28 0,-2-12 0,10 49 0,-2-5 0,-4-42 0,2 1 0,2-1 0,19 51 0,1 5 0,-19-56 0,41 132 0,46 146 0,-97-313 0,14 54 0,2-2 0,3 0 0,50 100 0,25 32 0,-47-88 0,-15-19 0,-29-66 0,2 0 0,0 0 0,1-1 0,0 0 0,1 0 0,1-1 0,15 20 0,-15-22 0,0 0 0,-1 1 0,0 0 0,-1 0 0,-1 1 0,6 15 0,-5-11 0,0-1 0,2 0 0,13 21 0,-2-8 0,21 44 0,7 12 0,-35-66 0,0 1 0,1-1 0,29 33 0,78 88 0,-29-48 0,-44-48 0,-37-36 0,0 0 0,-1 1 0,15 18 0,-16-18 0,0-1 0,0 0 0,0 0 0,19 11 0,20 19 0,-13-7 0,45 30 0,-3-3 0,5-3 0,-61-43 0,-1 0 0,34 28 0,3 0 0,-7-7 0,-27-17 0,1-1 0,34 18 0,-5-4 0,-22-13 0,0-2 0,2-2 0,-1 0 0,37 7 0,-53-15 0,-2-2 0,0 1 0,0 0 0,-1 2 0,19 8 0,-9-3 0,0-1 0,1-1 0,0-1 0,26 5 0,-21-6 0,-1 1 0,42 18 0,-37-12 0,1-2 0,55 13 0,-48-14 0,52 19 0,-54-16 0,80 16 0,-66-18 0,-52-12 0,13 3 0,1 1 0,-1 0 0,1 1 0,-1 1 0,15 8 0,-9-4 0,1-1 0,-1-1 0,43 10 0,-41-13 0,-1 1 0,0 1 0,-1 1 0,25 13 0,-20-8 0,0-2 0,1-1 0,40 11 0,32 12 0,131 40 0,-199-63 0,0-2 0,0 0 0,36 2 0,-60-9 0,150 18 0,-105-13 0,1-2 0,83-5 0,-50 0 0,-78 1 0,0 0 0,0-1 0,0 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,0 0 0,6-6 0,3-6 0,0 0 0,-1-1 0,19-28 0,4-7 0,-31 42 0,-1 0 0,0-1 0,0 1 0,-1-1 0,-1 0 0,0 0 0,0-1 0,-1 1 0,0-1 0,-1-17 0,1 9 0,1 0 0,6-24 0,1 6 0,8-75 0,-9 48 0,-2 3 0,-4 0 0,-5-85 0,-1 32 0,4 85 0,-1-1 0,-2 1 0,-1 0 0,-1 0 0,-2 1 0,0-1 0,-2 1 0,-2 1 0,0-1 0,-29-52 0,20 48 0,12 19 0,-1 0 0,-1 0 0,0 1 0,-13-15 0,-14-10 0,2 3 0,-44-57 0,69 81 0,1 1 0,-2 0 0,-12-10 0,-20-21 0,-61-64 0,11 13 0,62 59 0,-44-35 0,36 34 0,11 6 0,18 19 0,-1-1 0,1 2 0,-19-14 0,-26-17 0,-69-63 0,44 33 0,6-2 0,59 55 0,0 1 0,-2 0 0,0 1 0,0 1 0,-1 1 0,-22-13 0,4 10 0,25 11 0,1 0 0,0 0 0,0-1 0,0 0 0,0 0 0,1-1 0,-12-11 0,-25-27 0,3 1 0,-74-58 0,1 9 0,-78-62 0,137 108 0,-110-71 0,46 35 0,110 75 0,-127-102 0,62 46 0,45 40 0,-38-38 0,33 26 0,-44-32 0,46 40 0,-4-8 0,1-1 0,-45-58 0,26 28 0,11 11 0,20 25 0,-34-34 0,-21-18 0,-91-66 0,-40-16 0,29 30 0,146 109 0,-39-20 0,10 5 0,-68-34 0,124 70 0,0 1 0,-1 0 0,1 0 0,-1 1 0,1 0 0,-1 0 0,0 1 0,0 0 0,0 1 0,-12 0 0,7 0 0,0 0 0,0-1 0,-16-4 0,3-1 0,-52-3 0,-18-3 0,9-16 0,37 10 0,43 15 0,-1 1 0,1 0 0,-1 0 0,0 1 0,1 0 0,-1 1 0,0 0 0,0 0 0,0 1 0,0 0 0,1 0 0,-1 1 0,0 1 0,1-1 0,0 1 0,-1 0 0,-14 10 0,-14 6 0,27-15 0,0 1 0,0 1 0,1 0 0,-17 13 0,14-9-1365,1-1-5461</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-06-12T13:36:15.347"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">67 99 24575,'-1'0'0,"0"1"0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 2 0,-5 35 0,5-34 0,-4 63 0,8 100 0,-1-152 0,0-1 0,1 1 0,0-1 0,2 0 0,6 15 0,11 31 0,-13-27 0,2 0 0,1-1 0,1-1 0,21 33 0,61 107 0,28-5 0,-17-26 0,-98-128 0,1 0 0,21 18 0,15 19 0,-40-41 0,1-2 0,-1 1 0,1-1 0,11 8 0,-11-9 0,1 2 0,-1-1 0,1 1 0,6 9 0,-1 0 0,2-1 0,21 19 0,-20-19 0,0 0 0,17 22 0,12 17 0,3-2 0,67 57 0,-74-74 0,-18-15 0,36 37 0,-22-19 0,1-1 0,44 30 0,10 10 0,115 88 0,-120-100 0,147 94 0,-155-116 0,-52-30 0,37 24 0,-30-16 0,49 23 0,-23-14 0,23 7 0,-57-27 0,44 23 0,-43-18 0,54 19 0,-2-2 0,-28-10 0,1-2 0,59 13 0,-23-8 0,-24-3 0,-24-8 0,82 17 0,-41-9 0,-64-16 0,1-1 0,-1 0 0,36 4 0,32 2 0,14 0 0,85 13 0,-157-22 0,-1 1 0,0 2 0,25 7 0,-24-5 0,1-1 0,40 4 0,-9-5 0,67 16 0,-12-1 0,-12 2 0,-77-15 0,0-1 0,1-2 0,49 4 0,-36-6 0,47 7 0,-46-3 0,49 0 0,-17-5 0,109 15 0,-108-10 0,145-5 0,-95-3 0,-42 3 0,90-3 0,-147-2 0,0-1 0,-1-2 0,0 0 0,0-1 0,-1-2 0,0 0 0,0-1 0,29-21 0,-40 25 0,8-6 0,0-1 0,-2-1 0,0-1 0,27-33 0,4-2 0,-41 44 0,0-1 0,0 0 0,-1 0 0,0-1 0,-1 0 0,0 0 0,0 0 0,0-1 0,4-16 0,-5 10 0,0-1 0,-2 0 0,0 0 0,-1 0 0,-1-19 0,0-11 0,-8-125 0,5 149 0,-2-1 0,0 1 0,-1 0 0,-1 1 0,-14-30 0,-42-56 0,23 40 0,-1 8 0,-8-17 0,43 66 0,-1 0 0,0 1 0,-17-18 0,-4-5 0,-69-74 0,51 60 0,-9-12 0,36 37 0,0 1 0,-2 1 0,-45-34 0,1 1 0,31 26 0,-1 0 0,-42-22 0,37 25 0,-58-47 0,75 54 0,0 0 0,-25-12 0,0 0 0,-155-85 0,37 21 0,19 15 0,122 64 0,-1 1 0,-33-11 0,30 12 0,-43-22 0,32 14 0,-83-30 0,29 13 0,10 8 0,61 23 0,1-2 0,0 0 0,-31-17 0,34 15 0,-1 1 0,0 1 0,-25-7 0,24 9 0,0-1 0,0-1 0,-19-12 0,-126-53 0,145 63 0,-1 1 0,0 0 0,0 2 0,-27-5 0,24 6 0,0-1 0,0-1 0,-26-12 0,15 4 0,-2 2 0,0 1 0,-42-7 0,53 13 0,9 1 0,0 0 0,-26-14 0,27 12 0,-1 0 0,-27-8 0,-147-43 0,102 30 0,-228-52 0,248 59 0,55 15 0,0 2 0,-29-7 0,-342-71 0,90 33 0,293 49 0,-74-5 0,-136 6 0,89 2 0,90-2 0,3 1 0,0-1 0,0-2 0,-58-11 0,51 7 0,-1 1 0,1 2 0,-1 2 0,-51 4 0,-2 0 0,70-3 0,0 0 0,-31 6 0,43-4 0,0 1 0,1 0 0,-1 0 0,1 1 0,0 0 0,1 1 0,-16 10 0,-4 6 0,1 2 0,2 1 0,-27 30 0,19-19 0,28-30-114,-1 0 1,0 0-1,-1 0 0,1-1 0,-1 0 1,0 0-1,0 0 0,0-1 0,-1 0 1,1-1-1,-9 2 0,-1-1-6712</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2024-06-12T13:37:13.533"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0 24575,'0'0'-8191</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4050,8 +6178,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FAC2FE0-146B-4C91-950B-C1680CD19A41}">
   <dimension ref="B3:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>